<commit_message>
test sheets and examples
</commit_message>
<xml_diff>
--- a/www/SiteClassNameChecks/FolderNames.xlsx
+++ b/www/SiteClassNameChecks/FolderNames.xlsx
@@ -12,39 +12,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">ClassName</t>
   </si>
   <si>
-    <t xml:space="preserve">Applegate Ranger District</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blue Rock Pasture</t>
+    <t xml:space="preserve">Alakli Allotment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alkali Allotment</t>
   </si>
   <si>
     <t xml:space="preserve">Butler Butte Allotment</t>
   </si>
   <si>
-    <t xml:space="preserve">Cat Hill Pasture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conde  Creek Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deadwood Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliot Creek Allotment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Elliot Creek Allotment</t>
   </si>
   <si>
     <t xml:space="preserve">Fish Lake Allotment</t>
   </si>
   <si>
-    <t xml:space="preserve">Glade Creek Allotment</t>
+    <t xml:space="preserve">Hershberger Allotment</t>
   </si>
   <si>
     <t xml:space="preserve">High Cascade Ranger District</t>
@@ -53,40 +41,13 @@
     <t xml:space="preserve">High Cascades Ranger District</t>
   </si>
   <si>
-    <t xml:space="preserve">Imnaha Allotment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Local</t>
   </si>
   <si>
-    <t xml:space="preserve">P2 Pasture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P4 Pasture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Racheria Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rancharia Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rancheria Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red Blanket Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rogue Rive -Siskyou Ntional Forest National Forest</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rogue River-Siskiyou National Forests National Forest</t>
   </si>
   <si>
-    <t xml:space="preserve">Silver Beaver Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silver Meadow Allotment</t>
+    <t xml:space="preserve">Rouge River National Forest</t>
   </si>
   <si>
     <t xml:space="preserve">Siskiyou Mountains Ranger District</t>
@@ -95,31 +56,10 @@
     <t xml:space="preserve">Siskiyou Mountains Ranger District Ranger District</t>
   </si>
   <si>
-    <t xml:space="preserve">Siskiyou Mountains Ranger District/ High Cascade Ranger District</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tiller Ranger District</t>
   </si>
   <si>
-    <t xml:space="preserve">Tiller/ Prospect Ranger District</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unknown Allotment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unknown Pasture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upper Big Applegate Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wagner Butte Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wagner Mtn Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wickiup Meadow - Onion Spring Pasture</t>
   </si>
   <si>
     <t xml:space="preserve">Woodruff Allotment</t>
@@ -539,106 +479,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
backing up species replace lists
</commit_message>
<xml_diff>
--- a/www/SiteClassNameChecks/FolderNames.xlsx
+++ b/www/SiteClassNameChecks/FolderNames.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">ClassName</t>
   </si>
@@ -44,16 +44,13 @@
     <t xml:space="preserve">Local</t>
   </si>
   <si>
-    <t xml:space="preserve">Rogue River-Siskiyou National Forests National Forest</t>
+    <t xml:space="preserve">Rogue River-Siskiyou National Forest</t>
   </si>
   <si>
     <t xml:space="preserve">Rouge River National Forest</t>
   </si>
   <si>
     <t xml:space="preserve">Siskiyou Mountains Ranger District</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siskiyou Mountains Ranger District Ranger District</t>
   </si>
   <si>
     <t xml:space="preserve">Tiller Ranger District</t>
@@ -474,11 +471,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Update/backup of files created for testing
</commit_message>
<xml_diff>
--- a/www/SiteClassNameChecks/FolderNames.xlsx
+++ b/www/SiteClassNameChecks/FolderNames.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">ClassName</t>
   </si>
   <si>
-    <t xml:space="preserve">7N-Monitor Mesa Pasture</t>
+    <t xml:space="preserve">Alakli Allotment</t>
   </si>
   <si>
     <t xml:space="preserve">Alkali Allotment</t>
@@ -26,25 +26,67 @@
     <t xml:space="preserve">Big Grayback Allotment</t>
   </si>
   <si>
+    <t xml:space="preserve">Big Greyback Allotment</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bigelow Lakes Pasture</t>
   </si>
   <si>
+    <t xml:space="preserve">Butler Butte Allotment</t>
+  </si>
+  <si>
     <t xml:space="preserve">Crater Allotment</t>
   </si>
   <si>
+    <t xml:space="preserve">Elliot Creek Allotment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fish Lake Allotment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hershberger Allotment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Cascade Ranger District</t>
+  </si>
+  <si>
     <t xml:space="preserve">High Cascades Ranger District</t>
   </si>
   <si>
+    <t xml:space="preserve">Highcascades Ranger District</t>
+  </si>
+  <si>
     <t xml:space="preserve">Local</t>
   </si>
   <si>
+    <t xml:space="preserve">Moist Meadow Pasture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rogue River National Forest</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rogue River-Siskiyou National Forest</t>
   </si>
   <si>
+    <t xml:space="preserve">Rouge River National Forest</t>
+  </si>
+  <si>
     <t xml:space="preserve">Siskiyou Mountains Ranger District</t>
   </si>
   <si>
+    <t xml:space="preserve">Tiller Ranger District</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umpqua National Forest</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unknown Pasture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper Big Applegate Allotment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woodruff Allotment</t>
   </si>
 </sst>
 </file>
@@ -431,6 +473,76 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
update to Readme, add images - part 1
</commit_message>
<xml_diff>
--- a/www/SiteClassNameChecks/FolderNames.xlsx
+++ b/www/SiteClassNameChecks/FolderNames.xlsx
@@ -12,81 +12,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">ClassName</t>
   </si>
   <si>
-    <t xml:space="preserve">Alakli Allotment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Alkali Allotment</t>
   </si>
   <si>
     <t xml:space="preserve">Big Grayback Allotment</t>
   </si>
   <si>
-    <t xml:space="preserve">Big Greyback Allotment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bigelow Lakes Pasture</t>
   </si>
   <si>
-    <t xml:space="preserve">Butler Butte Allotment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Crater Allotment</t>
   </si>
   <si>
-    <t xml:space="preserve">Elliot Creek Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fish Lake Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hershberger Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High Cascade Ranger District</t>
-  </si>
-  <si>
     <t xml:space="preserve">High Cascades Ranger District</t>
   </si>
   <si>
-    <t xml:space="preserve">Highcascades Ranger District</t>
-  </si>
-  <si>
     <t xml:space="preserve">Local</t>
   </si>
   <si>
-    <t xml:space="preserve">Moist Meadow Pasture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rogue River National Forest</t>
+    <t xml:space="preserve">New Folder</t>
   </si>
   <si>
     <t xml:space="preserve">Rogue River-Siskiyou National Forest</t>
   </si>
   <si>
-    <t xml:space="preserve">Rouge River National Forest</t>
-  </si>
-  <si>
     <t xml:space="preserve">Siskiyou Mountains Ranger District</t>
   </si>
   <si>
-    <t xml:space="preserve">Tiller Ranger District</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Umpqua National Forest</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unknown Pasture</t>
   </si>
   <si>
     <t xml:space="preserve">Upper Big Applegate Allotment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woodruff Allotment</t>
   </si>
 </sst>
 </file>
@@ -478,71 +439,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>